<commit_message>
first pass of table codes
</commit_message>
<xml_diff>
--- a/sql/raw_data/2018microdata_codebook.xlsx
+++ b/sql/raw_data/2018microdata_codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evankuo/Desktop/Databases/EN.601.315-Databases-Final-Project/sql/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC998710-339A-1D4D-A572-23B510BCF640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73309BBB-CA77-B244-A258-E7A310EC9F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018 CBECS microdata codebook" sheetId="1" r:id="rId1"/>
@@ -10363,9 +10363,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1252"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A243" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B246" activeCellId="1" sqref="B247:B251 B246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>